<commit_message>
Start tab information construction
タブ情報構築開始
</commit_message>
<xml_diff>
--- a/document/個人_202109.xlsx
+++ b/document/個人_202109.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\users\hideo\Document2021\2021年\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\officinaWork\com.officina-hide.base\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBF5191-AC74-4468-AC92-DC971F32BA9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A2D1E4-35A0-4163-9398-BAAF6F291F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="18210" windowHeight="11505" activeTab="2" xr2:uid="{E445A735-B916-4613-9696-738E589472C3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="21996" windowHeight="13176" activeTab="1" xr2:uid="{E445A735-B916-4613-9696-738E589472C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="49">
   <si>
     <t>返済</t>
     <rPh sb="0" eb="2">
@@ -318,12 +318,23 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>氷、ドーナツ</t>
+    <rPh sb="0" eb="1">
+      <t>コオリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Loto</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -764,9 +775,9 @@
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15">
       <c r="B3">
         <v>8</v>
       </c>
@@ -781,7 +792,7 @@
         <v>108934</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15">
       <c r="D4">
         <v>11375</v>
       </c>
@@ -793,7 +804,7 @@
         <v>97559</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15">
       <c r="D5">
         <v>58032</v>
       </c>
@@ -809,7 +820,7 @@
         <v>1363.4666666666667</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15">
       <c r="D6">
         <v>13512</v>
       </c>
@@ -832,7 +843,7 @@
         <v>6215.75</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15">
       <c r="D7">
         <v>3200</v>
       </c>
@@ -852,7 +863,7 @@
         <v>6153.25</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15">
       <c r="B8">
         <v>9</v>
       </c>
@@ -881,7 +892,7 @@
         <v>6090.75</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15">
       <c r="D9">
         <v>20000</v>
       </c>
@@ -901,7 +912,7 @@
         <v>6028.25</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15">
       <c r="D10">
         <v>25000</v>
       </c>
@@ -921,7 +932,7 @@
         <v>5965.75</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15">
       <c r="D11">
         <v>24000</v>
       </c>
@@ -941,7 +952,7 @@
         <v>5903.25</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15">
       <c r="D12">
         <v>6215</v>
       </c>
@@ -964,7 +975,7 @@
         <v>5840.75</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15">
       <c r="D13">
         <v>58100</v>
       </c>
@@ -980,7 +991,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15">
       <c r="D14">
         <v>13400</v>
       </c>
@@ -996,7 +1007,7 @@
         <v>12916</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15">
       <c r="D15">
         <v>3200</v>
       </c>
@@ -1013,7 +1024,7 @@
         <v>12791</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15">
       <c r="B16">
         <v>10</v>
       </c>
@@ -1036,7 +1047,7 @@
         <v>12666</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11">
       <c r="C17">
         <v>80000</v>
       </c>
@@ -1052,7 +1063,7 @@
         <v>12541</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11">
       <c r="C18">
         <v>80000</v>
       </c>
@@ -1068,7 +1079,7 @@
         <v>12416</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11">
       <c r="D19">
         <v>100000</v>
       </c>
@@ -1081,7 +1092,7 @@
         <v>12291</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11">
       <c r="D20">
         <v>0</v>
       </c>
@@ -1098,7 +1109,7 @@
         <v>12166</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11">
       <c r="D21">
         <v>58100</v>
       </c>
@@ -1111,7 +1122,7 @@
         <v>12041</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11">
       <c r="D22">
         <v>13300</v>
       </c>
@@ -1128,7 +1139,7 @@
         <v>11916</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11">
       <c r="D23">
         <v>3200</v>
       </c>
@@ -1141,7 +1152,7 @@
         <v>11791</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11">
       <c r="B24">
         <v>11</v>
       </c>
@@ -1163,7 +1174,7 @@
         <v>11666</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11">
       <c r="D25">
         <v>20000</v>
       </c>
@@ -1176,7 +1187,7 @@
         <v>11541</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11">
       <c r="D26">
         <v>25000</v>
       </c>
@@ -1189,7 +1200,7 @@
         <v>11416</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11">
       <c r="D27">
         <v>0</v>
       </c>
@@ -1198,7 +1209,7 @@
         <v>210302</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11">
       <c r="D28">
         <v>6090</v>
       </c>
@@ -1211,7 +1222,7 @@
         <v>204212</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11">
       <c r="D29">
         <v>58100</v>
       </c>
@@ -1220,7 +1231,7 @@
         <v>146112</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11">
       <c r="D30">
         <v>13200</v>
       </c>
@@ -1233,7 +1244,7 @@
         <v>132912</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11">
       <c r="D31">
         <v>3200</v>
       </c>
@@ -1242,7 +1253,7 @@
         <v>129712</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11">
       <c r="B32">
         <v>12</v>
       </c>
@@ -1261,7 +1272,7 @@
         <v>277296</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6">
       <c r="D33">
         <v>20000</v>
       </c>
@@ -1270,7 +1281,7 @@
         <v>257296</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6">
       <c r="D34">
         <v>25000</v>
       </c>
@@ -1279,7 +1290,7 @@
         <v>232296</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6">
       <c r="D35">
         <v>0</v>
       </c>
@@ -1288,7 +1299,7 @@
         <v>232296</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6">
       <c r="D36">
         <v>6028</v>
       </c>
@@ -1301,7 +1312,7 @@
         <v>226268</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6">
       <c r="D37">
         <v>58100</v>
       </c>
@@ -1310,7 +1321,7 @@
         <v>168168</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:6">
       <c r="D38">
         <v>13100</v>
       </c>
@@ -1323,7 +1334,7 @@
         <v>155068</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:6">
       <c r="D39">
         <v>3200</v>
       </c>
@@ -1332,7 +1343,7 @@
         <v>151868</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:6">
       <c r="B40">
         <v>1</v>
       </c>
@@ -1351,7 +1362,7 @@
         <v>299577</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:6">
       <c r="D41">
         <v>20000</v>
       </c>
@@ -1360,7 +1371,7 @@
         <v>279577</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:6">
       <c r="D42">
         <v>25000</v>
       </c>
@@ -1369,7 +1380,7 @@
         <v>254577</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:6">
       <c r="D43">
         <v>0</v>
       </c>
@@ -1378,7 +1389,7 @@
         <v>254577</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:6">
       <c r="D44">
         <v>82000</v>
       </c>
@@ -1391,7 +1402,7 @@
         <v>172577</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:6">
       <c r="D45">
         <v>58100</v>
       </c>
@@ -1400,7 +1411,7 @@
         <v>114477</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:6">
       <c r="D46">
         <v>13000</v>
       </c>
@@ -1413,7 +1424,7 @@
         <v>101477</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:6">
       <c r="D47">
         <v>3200</v>
       </c>
@@ -1422,7 +1433,7 @@
         <v>98277</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:6">
       <c r="B48">
         <v>2</v>
       </c>
@@ -1441,7 +1452,7 @@
         <v>246111</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:6">
       <c r="D49">
         <v>20000</v>
       </c>
@@ -1450,7 +1461,7 @@
         <v>226111</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:6">
       <c r="D50">
         <v>25000</v>
       </c>
@@ -1459,7 +1470,7 @@
         <v>201111</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:6">
       <c r="D51">
         <v>0</v>
       </c>
@@ -1468,7 +1479,7 @@
         <v>201111</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:6">
       <c r="D52">
         <v>0</v>
       </c>
@@ -1481,7 +1492,7 @@
         <v>201111</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:6">
       <c r="D53">
         <v>58100</v>
       </c>
@@ -1490,7 +1501,7 @@
         <v>143011</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:6">
       <c r="D54">
         <v>12900</v>
       </c>
@@ -1503,7 +1514,7 @@
         <v>130111</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:6">
       <c r="B55">
         <v>3</v>
       </c>
@@ -1522,7 +1533,7 @@
         <v>278070</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:6">
       <c r="D56">
         <v>20000</v>
       </c>
@@ -1531,7 +1542,7 @@
         <v>258070</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:6">
       <c r="D57">
         <v>25000</v>
       </c>
@@ -1540,7 +1551,7 @@
         <v>233070</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:6">
       <c r="D58">
         <v>0</v>
       </c>
@@ -1549,7 +1560,7 @@
         <v>233070</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:6">
       <c r="D59">
         <v>0</v>
       </c>
@@ -1562,7 +1573,7 @@
         <v>233070</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:6">
       <c r="D60">
         <v>58100</v>
       </c>
@@ -1571,7 +1582,7 @@
         <v>174970</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:6">
       <c r="D61">
         <v>12800</v>
       </c>
@@ -1584,7 +1595,7 @@
         <v>162170</v>
       </c>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:6">
       <c r="D62">
         <v>3200</v>
       </c>
@@ -1593,7 +1604,7 @@
         <v>158970</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:6">
       <c r="B63">
         <v>4</v>
       </c>
@@ -1612,7 +1623,7 @@
         <v>307054</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:6">
       <c r="D64">
         <v>20000</v>
       </c>
@@ -1621,7 +1632,7 @@
         <v>287054</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:6">
       <c r="D65">
         <v>25000</v>
       </c>
@@ -1630,7 +1641,7 @@
         <v>262054</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:6">
       <c r="D66">
         <v>0</v>
       </c>
@@ -1639,7 +1650,7 @@
         <v>262054</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:6">
       <c r="D67">
         <v>0</v>
       </c>
@@ -1651,7 +1662,7 @@
         <v>262054</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:6">
       <c r="D68">
         <v>58100</v>
       </c>
@@ -1660,7 +1671,7 @@
         <v>203954</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:6">
       <c r="D69">
         <v>12700</v>
       </c>
@@ -1673,7 +1684,7 @@
         <v>191254</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:6">
       <c r="D70">
         <v>3200</v>
       </c>
@@ -1682,7 +1693,7 @@
         <v>188054</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:6">
       <c r="B71">
         <v>5</v>
       </c>
@@ -1701,7 +1712,7 @@
         <v>336263</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:6">
       <c r="D72">
         <v>20000</v>
       </c>
@@ -1710,7 +1721,7 @@
         <v>316263</v>
       </c>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:6">
       <c r="D73">
         <v>25000</v>
       </c>
@@ -1719,7 +1730,7 @@
         <v>291263</v>
       </c>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:6">
       <c r="D74">
         <v>0</v>
       </c>
@@ -1728,7 +1739,7 @@
         <v>291263</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:6">
       <c r="D75">
         <v>58100</v>
       </c>
@@ -1737,7 +1748,7 @@
         <v>233163</v>
       </c>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:6">
       <c r="D76">
         <v>12600</v>
       </c>
@@ -1750,7 +1761,7 @@
         <v>220563</v>
       </c>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:6">
       <c r="D77">
         <v>3200</v>
       </c>
@@ -1759,7 +1770,7 @@
         <v>217363</v>
       </c>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:6">
       <c r="B78">
         <v>6</v>
       </c>
@@ -1778,7 +1789,7 @@
         <v>247363</v>
       </c>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:6">
       <c r="D79">
         <v>20000</v>
       </c>
@@ -1787,7 +1798,7 @@
         <v>227363</v>
       </c>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:6">
       <c r="D80">
         <v>25000</v>
       </c>
@@ -1796,7 +1807,7 @@
         <v>202363</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:6">
       <c r="D81">
         <v>58100</v>
       </c>
@@ -1805,7 +1816,7 @@
         <v>144263</v>
       </c>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:6">
       <c r="D82">
         <v>12500</v>
       </c>
@@ -1818,7 +1829,7 @@
         <v>131763</v>
       </c>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:6">
       <c r="D83">
         <v>3200</v>
       </c>
@@ -1827,7 +1838,7 @@
         <v>128563</v>
       </c>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:6">
       <c r="B84">
         <v>7</v>
       </c>
@@ -1846,7 +1857,7 @@
         <v>288563</v>
       </c>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:6">
       <c r="D85">
         <v>20000</v>
       </c>
@@ -1855,7 +1866,7 @@
         <v>268563</v>
       </c>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:6">
       <c r="D86">
         <v>25000</v>
       </c>
@@ -1864,7 +1875,7 @@
         <v>243563</v>
       </c>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:6">
       <c r="D87">
         <v>58100</v>
       </c>
@@ -1873,7 +1884,7 @@
         <v>185463</v>
       </c>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:6">
       <c r="D88">
         <v>12400</v>
       </c>
@@ -1886,7 +1897,7 @@
         <v>173063</v>
       </c>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:6">
       <c r="D89">
         <v>3200</v>
       </c>
@@ -1895,7 +1906,7 @@
         <v>169863</v>
       </c>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:6">
       <c r="B90">
         <v>8</v>
       </c>
@@ -1910,7 +1921,7 @@
         <v>329863</v>
       </c>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:6">
       <c r="D91">
         <v>20000</v>
       </c>
@@ -1919,7 +1930,7 @@
         <v>309863</v>
       </c>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:6">
       <c r="D92">
         <v>25000</v>
       </c>
@@ -1928,7 +1939,7 @@
         <v>284863</v>
       </c>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:6">
       <c r="D93">
         <v>58100</v>
       </c>
@@ -1937,7 +1948,7 @@
         <v>226763</v>
       </c>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:6">
       <c r="D94">
         <v>12300</v>
       </c>
@@ -1950,7 +1961,7 @@
         <v>214463</v>
       </c>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:6">
       <c r="D95">
         <v>3200</v>
       </c>
@@ -1959,7 +1970,7 @@
         <v>211263</v>
       </c>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:6">
       <c r="B96">
         <v>9</v>
       </c>
@@ -1974,7 +1985,7 @@
         <v>351263</v>
       </c>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:6">
       <c r="D97">
         <v>25000</v>
       </c>
@@ -1983,7 +1994,7 @@
         <v>326263</v>
       </c>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:6">
       <c r="D98">
         <v>58100</v>
       </c>
@@ -1992,7 +2003,7 @@
         <v>268163</v>
       </c>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:6">
       <c r="D99">
         <v>12200</v>
       </c>
@@ -2005,7 +2016,7 @@
         <v>255963</v>
       </c>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:6">
       <c r="D100">
         <v>3200</v>
       </c>
@@ -2014,7 +2025,7 @@
         <v>252763</v>
       </c>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:6">
       <c r="B101">
         <v>10</v>
       </c>
@@ -2029,7 +2040,7 @@
         <v>392763</v>
       </c>
     </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:6">
       <c r="D102">
         <v>25000</v>
       </c>
@@ -2038,7 +2049,7 @@
         <v>367763</v>
       </c>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:6">
       <c r="D103">
         <v>58100</v>
       </c>
@@ -2047,7 +2058,7 @@
         <v>309663</v>
       </c>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:6">
       <c r="D104">
         <v>200000</v>
       </c>
@@ -2060,7 +2071,7 @@
         <v>109663</v>
       </c>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:6">
       <c r="D105">
         <v>3200</v>
       </c>
@@ -2069,7 +2080,7 @@
         <v>106463</v>
       </c>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:6">
       <c r="B106">
         <v>11</v>
       </c>
@@ -2084,7 +2095,7 @@
         <v>246463</v>
       </c>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:6">
       <c r="D107">
         <v>25000</v>
       </c>
@@ -2093,7 +2104,7 @@
         <v>221463</v>
       </c>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:6">
       <c r="D108">
         <v>58100</v>
       </c>
@@ -2102,7 +2113,7 @@
         <v>163363</v>
       </c>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:6">
       <c r="D109">
         <v>0</v>
       </c>
@@ -2115,7 +2126,7 @@
         <v>163363</v>
       </c>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:6">
       <c r="D110">
         <v>3200</v>
       </c>
@@ -2124,7 +2135,7 @@
         <v>160163</v>
       </c>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:6">
       <c r="B111">
         <v>12</v>
       </c>
@@ -2139,7 +2150,7 @@
         <v>300163</v>
       </c>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:6">
       <c r="D112">
         <v>25000</v>
       </c>
@@ -2148,7 +2159,7 @@
         <v>275163</v>
       </c>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:6">
       <c r="D113">
         <v>58100</v>
       </c>
@@ -2157,7 +2168,7 @@
         <v>217063</v>
       </c>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:6">
       <c r="D114">
         <v>0</v>
       </c>
@@ -2166,7 +2177,7 @@
         <v>217063</v>
       </c>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:6">
       <c r="D115">
         <v>3200</v>
       </c>
@@ -2175,7 +2186,7 @@
         <v>213863</v>
       </c>
     </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:6">
       <c r="B116">
         <v>1</v>
       </c>
@@ -2190,7 +2201,7 @@
         <v>353863</v>
       </c>
     </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:6">
       <c r="D117">
         <v>25000</v>
       </c>
@@ -2199,7 +2210,7 @@
         <v>328863</v>
       </c>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:6">
       <c r="D118">
         <v>58100</v>
       </c>
@@ -2208,7 +2219,7 @@
         <v>270763</v>
       </c>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:6">
       <c r="D119">
         <v>3200</v>
       </c>
@@ -2217,7 +2228,7 @@
         <v>267563</v>
       </c>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:6">
       <c r="B120">
         <v>2</v>
       </c>
@@ -2232,7 +2243,7 @@
         <v>407563</v>
       </c>
     </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:6">
       <c r="D121">
         <v>25000</v>
       </c>
@@ -2241,7 +2252,7 @@
         <v>382563</v>
       </c>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:6">
       <c r="D122">
         <v>58100</v>
       </c>
@@ -2250,7 +2261,7 @@
         <v>324463</v>
       </c>
     </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:6">
       <c r="D123">
         <v>3200</v>
       </c>
@@ -2259,7 +2270,7 @@
         <v>321263</v>
       </c>
     </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:6">
       <c r="B124">
         <v>3</v>
       </c>
@@ -2274,7 +2285,7 @@
         <v>461263</v>
       </c>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:6">
       <c r="D125">
         <v>25000</v>
       </c>
@@ -2283,7 +2294,7 @@
         <v>436263</v>
       </c>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:6">
       <c r="D126">
         <v>58100</v>
       </c>
@@ -2292,7 +2303,7 @@
         <v>378163</v>
       </c>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:6">
       <c r="D127">
         <v>3200</v>
       </c>
@@ -2301,7 +2312,7 @@
         <v>374963</v>
       </c>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:6">
       <c r="B128">
         <v>4</v>
       </c>
@@ -2316,7 +2327,7 @@
         <v>514963</v>
       </c>
     </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:6">
       <c r="D129">
         <v>25000</v>
       </c>
@@ -2325,7 +2336,7 @@
         <v>489963</v>
       </c>
     </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:6">
       <c r="D130">
         <v>58100</v>
       </c>
@@ -2334,7 +2345,7 @@
         <v>431863</v>
       </c>
     </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:6">
       <c r="D131">
         <v>3200</v>
       </c>
@@ -2343,7 +2354,7 @@
         <v>428663</v>
       </c>
     </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:6">
       <c r="B132">
         <v>5</v>
       </c>
@@ -2358,7 +2369,7 @@
         <v>568663</v>
       </c>
     </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:6">
       <c r="D133">
         <v>25000</v>
       </c>
@@ -2367,7 +2378,7 @@
         <v>543663</v>
       </c>
     </row>
-    <row r="134" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:6">
       <c r="D134">
         <v>58100</v>
       </c>
@@ -2376,7 +2387,7 @@
         <v>485563</v>
       </c>
     </row>
-    <row r="135" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:6">
       <c r="D135">
         <v>3200</v>
       </c>
@@ -2385,7 +2396,7 @@
         <v>482363</v>
       </c>
     </row>
-    <row r="136" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:6">
       <c r="B136">
         <v>6</v>
       </c>
@@ -2400,7 +2411,7 @@
         <v>622363</v>
       </c>
     </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:6">
       <c r="D137">
         <v>25000</v>
       </c>
@@ -2409,7 +2420,7 @@
         <v>597363</v>
       </c>
     </row>
-    <row r="138" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:6">
       <c r="D138">
         <v>58100</v>
       </c>
@@ -2418,7 +2429,7 @@
         <v>539263</v>
       </c>
     </row>
-    <row r="139" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:6">
       <c r="D139">
         <v>3200</v>
       </c>
@@ -2427,7 +2438,7 @@
         <v>536063</v>
       </c>
     </row>
-    <row r="140" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:6">
       <c r="B140">
         <v>7</v>
       </c>
@@ -2442,7 +2453,7 @@
         <v>676063</v>
       </c>
     </row>
-    <row r="141" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:6">
       <c r="D141">
         <v>25000</v>
       </c>
@@ -2451,7 +2462,7 @@
         <v>651063</v>
       </c>
     </row>
-    <row r="142" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:6">
       <c r="D142">
         <v>58100</v>
       </c>
@@ -2460,7 +2471,7 @@
         <v>592963</v>
       </c>
     </row>
-    <row r="143" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:6">
       <c r="D143">
         <v>3200</v>
       </c>
@@ -2469,7 +2480,7 @@
         <v>589763</v>
       </c>
     </row>
-    <row r="144" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:6">
       <c r="B144">
         <v>8</v>
       </c>
@@ -2484,7 +2495,7 @@
         <v>729763</v>
       </c>
     </row>
-    <row r="145" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="4:6">
       <c r="D145">
         <v>25000</v>
       </c>
@@ -2493,7 +2504,7 @@
         <v>704763</v>
       </c>
     </row>
-    <row r="146" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="4:6">
       <c r="D146">
         <v>58100</v>
       </c>
@@ -2502,7 +2513,7 @@
         <v>646663</v>
       </c>
     </row>
-    <row r="147" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="4:6">
       <c r="D147">
         <v>3200</v>
       </c>
@@ -2519,29 +2530,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E68EDCEE-DBDF-4D86-B0FF-D8A39D458466}">
-  <dimension ref="B2:L62"/>
+  <dimension ref="B2:L63"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="3.5" customWidth="1"/>
-    <col min="5" max="5" width="9.875" customWidth="1"/>
-    <col min="6" max="8" width="8.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="8.75" style="7"/>
+    <col min="2" max="2" width="5.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="3.453125" customWidth="1"/>
+    <col min="5" max="5" width="9.90625" customWidth="1"/>
+    <col min="6" max="8" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.36328125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7265625" style="7"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12">
       <c r="H2" s="1">
         <v>32850</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12">
       <c r="B3">
         <v>2021</v>
       </c>
@@ -2559,7 +2570,7 @@
         <v>192850</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12">
       <c r="D4">
         <v>26</v>
       </c>
@@ -2570,7 +2581,7 @@
         <v>20000</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" ref="H4:H62" si="0">H3+F4-G4</f>
+        <f t="shared" ref="H4:H63" si="0">H3+F4-G4</f>
         <v>172850</v>
       </c>
       <c r="J4" s="1">
@@ -2581,7 +2592,7 @@
         <v>80550</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12">
       <c r="D5">
         <v>27</v>
       </c>
@@ -2603,7 +2614,7 @@
         <v>65954</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12">
       <c r="D6">
         <v>27</v>
       </c>
@@ -2622,7 +2633,7 @@
       </c>
       <c r="L6" s="9"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12">
       <c r="D7">
         <v>29</v>
       </c>
@@ -2638,7 +2649,7 @@
       </c>
       <c r="L7" s="10"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12">
       <c r="C8">
         <v>9</v>
       </c>
@@ -2660,7 +2671,7 @@
       </c>
       <c r="L8" s="10"/>
     </row>
-    <row r="9" spans="2:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" s="4" customFormat="1">
       <c r="D9" s="4">
         <v>2</v>
       </c>
@@ -2681,7 +2692,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="10"/>
     </row>
-    <row r="10" spans="2:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" s="4" customFormat="1">
       <c r="D10" s="4">
         <v>9</v>
       </c>
@@ -2700,7 +2711,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="10"/>
     </row>
-    <row r="11" spans="2:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" s="10" customFormat="1">
       <c r="D11" s="10">
         <v>10</v>
       </c>
@@ -2720,7 +2731,7 @@
       </c>
       <c r="K11" s="11"/>
     </row>
-    <row r="12" spans="2:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" s="10" customFormat="1">
       <c r="D12" s="10">
         <v>10</v>
       </c>
@@ -2740,7 +2751,7 @@
       </c>
       <c r="K12" s="11"/>
     </row>
-    <row r="13" spans="2:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" s="10" customFormat="1">
       <c r="D13" s="10">
         <v>11</v>
       </c>
@@ -2751,16 +2762,16 @@
         <v>8000</v>
       </c>
       <c r="G13" s="11">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="H13" s="5">
         <f t="shared" si="0"/>
-        <v>26080</v>
+        <v>25080</v>
       </c>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
     </row>
-    <row r="14" spans="2:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" s="10" customFormat="1">
       <c r="E14" s="10" t="s">
         <v>2</v>
       </c>
@@ -2770,737 +2781,744 @@
       </c>
       <c r="H14" s="5">
         <f t="shared" si="0"/>
-        <v>24080</v>
+        <v>23080</v>
       </c>
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2">
-        <v>24</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3">
-        <v>160000</v>
-      </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3">
-        <f t="shared" si="0"/>
-        <v>184080</v>
-      </c>
-      <c r="I15" s="7"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" s="10" customFormat="1">
+      <c r="D15" s="10">
+        <v>13</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11">
+        <v>600</v>
+      </c>
+      <c r="H15" s="5">
+        <f t="shared" si="0"/>
+        <v>22480</v>
+      </c>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+    </row>
+    <row r="16" spans="2:12">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2">
         <v>24</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3">
-        <v>20000</v>
-      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="3">
+        <v>160000</v>
+      </c>
+      <c r="G16" s="3"/>
       <c r="H16" s="3">
         <f t="shared" si="0"/>
-        <v>164080</v>
+        <v>182480</v>
       </c>
       <c r="I16" s="7"/>
-      <c r="J16" s="3">
-        <f>J4-K16</f>
-        <v>911450</v>
-      </c>
-      <c r="K16" s="3">
-        <v>8000</v>
-      </c>
-      <c r="L16" s="8">
-        <f>1000000-J16</f>
-        <v>88550</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="2:12">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3">
-        <v>25000</v>
+        <v>20000</v>
       </c>
       <c r="H17" s="3">
         <f t="shared" si="0"/>
-        <v>139080</v>
+        <v>162480</v>
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="3">
-        <f>J5-K17</f>
-        <v>1926046</v>
+        <f>J4-K17</f>
+        <v>911450</v>
       </c>
       <c r="K17" s="3">
         <v>8000</v>
       </c>
       <c r="L17" s="8">
-        <f>2000000-J17</f>
-        <v>73954</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+        <f>1000000-J17</f>
+        <v>88550</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3">
-        <v>3200</v>
+        <v>25000</v>
       </c>
       <c r="H18" s="3">
-        <f>H13+F18-G18</f>
-        <v>22880</v>
+        <f t="shared" si="0"/>
+        <v>137480</v>
       </c>
       <c r="I18" s="7"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J18" s="3">
+        <f>J5-K18</f>
+        <v>1926046</v>
+      </c>
+      <c r="K18" s="3">
+        <v>8000</v>
+      </c>
+      <c r="L18" s="8">
+        <f>2000000-J18</f>
+        <v>73954</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3">
-        <v>12791</v>
+        <v>3200</v>
       </c>
       <c r="H19" s="3">
-        <f>H17+F19-G19</f>
-        <v>126289</v>
+        <f>H13+F19-G19</f>
+        <v>21880</v>
       </c>
       <c r="I19" s="7"/>
-      <c r="J19" s="3">
-        <f>J6-K19</f>
-        <v>213343</v>
-      </c>
-      <c r="K19" s="3">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="2:12">
       <c r="B20" s="2"/>
-      <c r="C20" s="2">
-        <v>9</v>
-      </c>
+      <c r="C20" s="2"/>
       <c r="D20" s="2">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3">
-        <v>24300</v>
+        <v>12791</v>
       </c>
       <c r="H20" s="3">
-        <f t="shared" si="0"/>
-        <v>101989</v>
+        <f>H18+F20-G20</f>
+        <v>124689</v>
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="3">
-        <v>168000</v>
-      </c>
-      <c r="K20" s="3"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+        <f>J6-K20</f>
+        <v>213343</v>
+      </c>
+      <c r="K20" s="3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12">
       <c r="B21" s="2"/>
       <c r="C21" s="2">
+        <v>9</v>
+      </c>
+      <c r="D21" s="2">
+        <v>31</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3">
+        <v>24300</v>
+      </c>
+      <c r="H21" s="3">
+        <f t="shared" si="0"/>
+        <v>100389</v>
+      </c>
+      <c r="I21" s="7"/>
+      <c r="J21" s="3">
+        <v>168000</v>
+      </c>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="2:12">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2">
         <v>10</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D22" s="2">
         <v>2</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="3">
-        <v>40000</v>
-      </c>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3">
-        <f t="shared" si="0"/>
-        <v>141989</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J21" s="3">
-        <f>J16-K21</f>
-        <v>951450</v>
-      </c>
-      <c r="K21" s="3">
-        <v>-40000</v>
-      </c>
-      <c r="L21" s="8">
-        <f>1000000-J21</f>
-        <v>48550</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="3">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3">
         <f t="shared" si="0"/>
-        <v>161989</v>
+        <v>130389</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J22" s="3">
         <f>J17-K22</f>
-        <v>1946046</v>
+        <v>941450</v>
       </c>
       <c r="K22" s="3">
-        <v>-20000</v>
+        <v>-30000</v>
       </c>
       <c r="L22" s="8">
-        <f>2000000-J22</f>
-        <v>53954</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+        <f>1000000-J22</f>
+        <v>58550</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3">
-        <v>94411</v>
-      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="3">
+        <v>40000</v>
+      </c>
+      <c r="G23" s="3"/>
       <c r="H23" s="3">
         <f t="shared" si="0"/>
-        <v>67578</v>
-      </c>
-      <c r="I23" s="7"/>
+        <v>170389</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="J23" s="3">
-        <v>0</v>
-      </c>
-      <c r="K23" s="3"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+        <f>J18-K23</f>
+        <v>1966046</v>
+      </c>
+      <c r="K23" s="3">
+        <v>-40000</v>
+      </c>
+      <c r="L23" s="8">
+        <f>2000000-J23</f>
+        <v>33954</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="2">
-        <v>10</v>
-      </c>
+      <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3">
-        <v>58100</v>
+        <v>94411</v>
       </c>
       <c r="H24" s="3">
         <f t="shared" si="0"/>
-        <v>9478</v>
+        <v>75978</v>
       </c>
       <c r="I24" s="7"/>
-      <c r="J24" s="3"/>
+      <c r="J24" s="3">
+        <v>0</v>
+      </c>
       <c r="K24" s="3"/>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2">
+        <v>10</v>
+      </c>
       <c r="E25" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3">
-        <v>13612</v>
+        <v>58100</v>
       </c>
       <c r="H25" s="3">
         <f t="shared" si="0"/>
-        <v>-4134</v>
+        <v>17878</v>
       </c>
       <c r="I25" s="7"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="2">
-        <v>25</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="3">
-        <v>160000</v>
-      </c>
-      <c r="G26" s="3"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3">
+        <v>13612</v>
+      </c>
       <c r="H26" s="3">
         <f t="shared" si="0"/>
-        <v>155866</v>
+        <v>4266</v>
       </c>
       <c r="I26" s="7"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2">
-        <v>26</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3">
-        <v>3200</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="3">
+        <v>160000</v>
+      </c>
+      <c r="G27" s="3"/>
       <c r="H27" s="3">
         <f t="shared" si="0"/>
-        <v>152666</v>
+        <v>164266</v>
       </c>
       <c r="I27" s="7"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3">
-        <v>25000</v>
+        <v>3200</v>
       </c>
       <c r="H28" s="3">
         <f t="shared" si="0"/>
-        <v>127666</v>
+        <v>161066</v>
       </c>
       <c r="I28" s="7"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+      <c r="D29" s="2">
+        <v>27</v>
+      </c>
       <c r="E29" s="2" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3">
-        <v>20000</v>
+        <v>25000</v>
       </c>
       <c r="H29" s="3">
         <f t="shared" si="0"/>
-        <v>107666</v>
+        <v>136066</v>
       </c>
       <c r="I29" s="7"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D30" s="2">
+    <row r="30" spans="2:12">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="F30" s="3"/>
+      <c r="G30" s="3">
+        <v>20000</v>
+      </c>
+      <c r="H30" s="3">
+        <f t="shared" si="0"/>
+        <v>116066</v>
+      </c>
+      <c r="I30" s="7"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+    </row>
+    <row r="31" spans="2:12">
+      <c r="D31" s="2">
+        <v>31</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G30" s="6">
+      <c r="G31" s="6">
         <v>24000</v>
       </c>
-      <c r="H30" s="3">
-        <f t="shared" si="0"/>
-        <v>83666</v>
-      </c>
-      <c r="I30" s="7"/>
-      <c r="J30" s="3">
+      <c r="H31" s="3">
+        <f t="shared" si="0"/>
+        <v>92066</v>
+      </c>
+      <c r="I31" s="7"/>
+      <c r="J31" s="3">
         <v>144000</v>
       </c>
-      <c r="K30" s="3"/>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D31" s="2">
+      <c r="K31" s="3"/>
+    </row>
+    <row r="32" spans="2:12">
+      <c r="C32">
+        <v>11</v>
+      </c>
+      <c r="D32" s="2">
         <v>10</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G31" s="6">
+      <c r="G32" s="6">
         <v>58100</v>
       </c>
-      <c r="H31" s="3">
-        <f t="shared" si="0"/>
-        <v>25566</v>
-      </c>
-      <c r="I31" s="7"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E32" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G32" s="6">
-        <v>13500</v>
-      </c>
       <c r="H32" s="3">
         <f t="shared" si="0"/>
-        <v>12066</v>
+        <v>33966</v>
       </c>
       <c r="I32" s="7"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
     </row>
-    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="D33" s="7">
-        <v>25</v>
-      </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="3">
-        <v>160000</v>
-      </c>
-      <c r="G33" s="3"/>
+    <row r="33" spans="3:11">
+      <c r="E33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="6">
+        <v>13500</v>
+      </c>
       <c r="H33" s="3">
         <f t="shared" si="0"/>
-        <v>172066</v>
+        <v>20466</v>
       </c>
       <c r="I33" s="7"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
     </row>
-    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="D34" s="7"/>
-      <c r="E34" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3">
-        <v>20000</v>
-      </c>
+    <row r="34" spans="3:11">
+      <c r="D34" s="7">
+        <v>25</v>
+      </c>
+      <c r="E34" s="7"/>
+      <c r="F34" s="3">
+        <v>160000</v>
+      </c>
+      <c r="G34" s="3"/>
       <c r="H34" s="3">
         <f t="shared" si="0"/>
-        <v>152066</v>
+        <v>180466</v>
       </c>
       <c r="I34" s="7"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
     </row>
-    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="D35" s="7">
-        <v>26</v>
-      </c>
+    <row r="35" spans="3:11">
+      <c r="D35" s="7"/>
       <c r="E35" s="7" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3">
-        <v>3200</v>
+        <v>20000</v>
       </c>
       <c r="H35" s="3">
         <f t="shared" si="0"/>
-        <v>148866</v>
+        <v>160466</v>
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
     </row>
-    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:11">
       <c r="D36" s="7">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3">
-        <v>25000</v>
+        <v>3200</v>
       </c>
       <c r="H36" s="3">
         <f t="shared" si="0"/>
-        <v>123866</v>
+        <v>157266</v>
       </c>
       <c r="I36" s="7"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
     </row>
-    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="D37" s="7"/>
+    <row r="37" spans="3:11">
+      <c r="D37" s="7">
+        <v>27</v>
+      </c>
       <c r="E37" s="7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3">
-        <v>12666</v>
+        <v>25000</v>
       </c>
       <c r="H37" s="3">
         <f t="shared" si="0"/>
-        <v>111200</v>
+        <v>132266</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
     </row>
-    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="D38" s="7">
-        <v>30</v>
-      </c>
+    <row r="38" spans="3:11">
+      <c r="D38" s="7"/>
       <c r="E38" s="7" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3">
-        <v>24000</v>
+        <v>12666</v>
       </c>
       <c r="H38" s="3">
         <f t="shared" si="0"/>
-        <v>87200</v>
+        <v>119600</v>
       </c>
       <c r="I38" s="7"/>
-      <c r="J38" s="3">
-        <v>120000</v>
-      </c>
+      <c r="J38" s="3"/>
       <c r="K38" s="3"/>
     </row>
-    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C39" s="2">
+    <row r="39" spans="3:11">
+      <c r="D39" s="7">
+        <v>30</v>
+      </c>
+      <c r="E39" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="D39" s="7">
-        <v>10</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>12</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3">
-        <v>58100</v>
+        <v>24000</v>
       </c>
       <c r="H39" s="3">
         <f t="shared" si="0"/>
-        <v>29100</v>
+        <v>95600</v>
       </c>
       <c r="I39" s="7"/>
-      <c r="J39" s="3"/>
+      <c r="J39" s="3">
+        <v>120000</v>
+      </c>
       <c r="K39" s="3"/>
     </row>
-    <row r="40" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C40" s="2"/>
-      <c r="D40" s="7"/>
+    <row r="40" spans="3:11">
+      <c r="C40" s="2">
+        <v>12</v>
+      </c>
+      <c r="D40" s="7">
+        <v>10</v>
+      </c>
       <c r="E40" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="3">
-        <v>13400</v>
+        <v>58100</v>
       </c>
       <c r="H40" s="3">
         <f t="shared" si="0"/>
-        <v>15700</v>
+        <v>37500</v>
       </c>
       <c r="I40" s="7"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
     </row>
-    <row r="41" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:11">
       <c r="C41" s="2"/>
-      <c r="D41" s="7">
-        <v>23</v>
-      </c>
+      <c r="D41" s="7"/>
       <c r="E41" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3">
-        <v>3200</v>
+        <v>13400</v>
       </c>
       <c r="H41" s="3">
         <f t="shared" si="0"/>
-        <v>12500</v>
+        <v>24100</v>
       </c>
       <c r="I41" s="7"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
     </row>
-    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:11">
       <c r="C42" s="2"/>
       <c r="D42" s="7">
-        <v>25</v>
-      </c>
-      <c r="E42" s="7"/>
-      <c r="F42" s="3">
-        <v>160000</v>
-      </c>
-      <c r="G42" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3">
+        <v>3200</v>
+      </c>
       <c r="H42" s="3">
         <f t="shared" si="0"/>
-        <v>172500</v>
+        <v>20900</v>
       </c>
       <c r="I42" s="7"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
     </row>
-    <row r="43" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:11">
       <c r="C43" s="2"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3">
-        <v>20000</v>
-      </c>
+      <c r="D43" s="7">
+        <v>25</v>
+      </c>
+      <c r="E43" s="7"/>
+      <c r="F43" s="3">
+        <v>160000</v>
+      </c>
+      <c r="G43" s="3"/>
       <c r="H43" s="3">
         <f t="shared" si="0"/>
-        <v>152500</v>
+        <v>180900</v>
       </c>
       <c r="I43" s="7"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
     </row>
-    <row r="44" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:11">
       <c r="C44" s="2"/>
-      <c r="D44" s="7">
-        <v>28</v>
-      </c>
+      <c r="D44" s="7"/>
       <c r="E44" s="7" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3">
-        <v>25000</v>
+        <v>20000</v>
       </c>
       <c r="H44" s="3">
         <f t="shared" si="0"/>
-        <v>127500</v>
+        <v>160900</v>
       </c>
       <c r="I44" s="7"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
     </row>
-    <row r="45" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:11">
       <c r="C45" s="2"/>
-      <c r="D45" s="7"/>
+      <c r="D45" s="7">
+        <v>28</v>
+      </c>
       <c r="E45" s="7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3">
-        <v>12541</v>
+        <v>25000</v>
       </c>
       <c r="H45" s="3">
         <f t="shared" si="0"/>
-        <v>114959</v>
+        <v>135900</v>
       </c>
       <c r="I45" s="7"/>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
     </row>
-    <row r="46" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:11">
       <c r="C46" s="2"/>
-      <c r="D46" s="7">
-        <v>30</v>
-      </c>
+      <c r="D46" s="7"/>
       <c r="E46" s="7" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3">
-        <v>24000</v>
+        <v>12541</v>
       </c>
       <c r="H46" s="3">
         <f t="shared" si="0"/>
-        <v>90959</v>
+        <v>123359</v>
       </c>
       <c r="I46" s="7"/>
-      <c r="J46" s="3">
-        <v>96000</v>
-      </c>
+      <c r="J46" s="3"/>
       <c r="K46" s="3"/>
     </row>
-    <row r="47" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C47" s="7">
-        <v>12</v>
-      </c>
+    <row r="47" spans="3:11">
+      <c r="C47" s="2"/>
       <c r="D47" s="7">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3">
-        <v>58100</v>
+        <v>24000</v>
       </c>
       <c r="H47" s="3">
         <f t="shared" si="0"/>
-        <v>32859</v>
+        <v>99359</v>
       </c>
       <c r="I47" s="7"/>
-      <c r="J47" s="3"/>
+      <c r="J47" s="3">
+        <v>96000</v>
+      </c>
       <c r="K47" s="3"/>
     </row>
-    <row r="48" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
+    <row r="48" spans="3:11">
+      <c r="C48" s="7">
+        <v>1</v>
+      </c>
+      <c r="D48" s="7">
+        <v>10</v>
+      </c>
       <c r="E48" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3">
-        <v>12400</v>
+        <v>58100</v>
       </c>
       <c r="H48" s="3">
         <f t="shared" si="0"/>
-        <v>20459</v>
+        <v>41259</v>
       </c>
       <c r="I48" s="7"/>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
     </row>
-    <row r="49" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:11">
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
+      <c r="E49" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
+      <c r="G49" s="3">
+        <v>12400</v>
+      </c>
       <c r="H49" s="3">
         <f t="shared" si="0"/>
-        <v>20459</v>
+        <v>28859</v>
       </c>
       <c r="I49" s="7"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
     </row>
-    <row r="50" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:11">
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="7"/>
@@ -3508,13 +3526,13 @@
       <c r="G50" s="3"/>
       <c r="H50" s="3">
         <f t="shared" si="0"/>
-        <v>20459</v>
+        <v>28859</v>
       </c>
       <c r="I50" s="7"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
     </row>
-    <row r="51" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:11">
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
@@ -3522,13 +3540,13 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3">
         <f t="shared" si="0"/>
-        <v>20459</v>
+        <v>28859</v>
       </c>
       <c r="I51" s="7"/>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
     </row>
-    <row r="52" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:11">
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="7"/>
@@ -3536,13 +3554,13 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3">
         <f t="shared" si="0"/>
-        <v>20459</v>
+        <v>28859</v>
       </c>
       <c r="I52" s="7"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
     </row>
-    <row r="53" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:11">
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
@@ -3550,13 +3568,13 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3">
         <f t="shared" si="0"/>
-        <v>20459</v>
+        <v>28859</v>
       </c>
       <c r="I53" s="7"/>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
     </row>
-    <row r="54" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:11">
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
       <c r="E54" s="7"/>
@@ -3564,13 +3582,13 @@
       <c r="G54" s="3"/>
       <c r="H54" s="3">
         <f t="shared" si="0"/>
-        <v>20459</v>
+        <v>28859</v>
       </c>
       <c r="I54" s="7"/>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
     </row>
-    <row r="55" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:11">
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
@@ -3578,13 +3596,13 @@
       <c r="G55" s="3"/>
       <c r="H55" s="3">
         <f t="shared" si="0"/>
-        <v>20459</v>
+        <v>28859</v>
       </c>
       <c r="I55" s="7"/>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
     </row>
-    <row r="56" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:11">
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
       <c r="E56" s="7"/>
@@ -3592,13 +3610,13 @@
       <c r="G56" s="3"/>
       <c r="H56" s="3">
         <f t="shared" si="0"/>
-        <v>20459</v>
+        <v>28859</v>
       </c>
       <c r="I56" s="7"/>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
     </row>
-    <row r="57" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:11">
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
       <c r="E57" s="7"/>
@@ -3606,13 +3624,13 @@
       <c r="G57" s="3"/>
       <c r="H57" s="3">
         <f t="shared" si="0"/>
-        <v>20459</v>
+        <v>28859</v>
       </c>
       <c r="I57" s="7"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
     </row>
-    <row r="58" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:11">
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="7"/>
@@ -3620,13 +3638,13 @@
       <c r="G58" s="3"/>
       <c r="H58" s="3">
         <f t="shared" si="0"/>
-        <v>20459</v>
+        <v>28859</v>
       </c>
       <c r="I58" s="7"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
     </row>
-    <row r="59" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:11">
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="7"/>
@@ -3634,13 +3652,13 @@
       <c r="G59" s="3"/>
       <c r="H59" s="3">
         <f t="shared" si="0"/>
-        <v>20459</v>
+        <v>28859</v>
       </c>
       <c r="I59" s="7"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
     </row>
-    <row r="60" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:11">
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="7"/>
@@ -3648,13 +3666,13 @@
       <c r="G60" s="3"/>
       <c r="H60" s="3">
         <f t="shared" si="0"/>
-        <v>20459</v>
+        <v>28859</v>
       </c>
       <c r="I60" s="7"/>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
     </row>
-    <row r="61" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:11">
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
@@ -3662,13 +3680,13 @@
       <c r="G61" s="3"/>
       <c r="H61" s="3">
         <f t="shared" si="0"/>
-        <v>20459</v>
+        <v>28859</v>
       </c>
       <c r="I61" s="7"/>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
     </row>
-    <row r="62" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:11">
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="7"/>
@@ -3676,11 +3694,25 @@
       <c r="G62" s="3"/>
       <c r="H62" s="3">
         <f t="shared" si="0"/>
-        <v>20459</v>
+        <v>28859</v>
       </c>
       <c r="I62" s="7"/>
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
+    </row>
+    <row r="63" spans="3:11">
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3">
+        <f t="shared" si="0"/>
+        <v>28859</v>
+      </c>
+      <c r="I63" s="7"/>
+      <c r="J63" s="3"/>
+      <c r="K63" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -3693,19 +3725,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB6879B4-F831-485C-A8C8-6EB57659B6DE}">
   <dimension ref="A2:N114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="3.5" customWidth="1"/>
-    <col min="6" max="6" width="12.5" customWidth="1"/>
-    <col min="7" max="12" width="8.75" style="1"/>
+    <col min="2" max="2" width="5.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="3.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" customWidth="1"/>
+    <col min="7" max="12" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
@@ -3719,7 +3751,7 @@
         <v>1854</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="B3">
         <v>2021</v>
       </c>
@@ -3747,7 +3779,7 @@
         <v>1854</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="D4">
         <v>2</v>
       </c>
@@ -3769,7 +3801,7 @@
         <v>1854</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="10" customFormat="1">
       <c r="F5" s="10" t="s">
         <v>20</v>
       </c>
@@ -3788,7 +3820,7 @@
         <v>1854</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" s="10" customFormat="1">
       <c r="D6" s="10">
         <v>3</v>
       </c>
@@ -3815,7 +3847,7 @@
         <v>1754</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="10" customFormat="1">
       <c r="F7" s="10" t="s">
         <v>21</v>
       </c>
@@ -3834,7 +3866,7 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="10" customFormat="1">
       <c r="F8" s="10" t="s">
         <v>32</v>
       </c>
@@ -3853,7 +3885,7 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="10" customFormat="1">
       <c r="F9" s="10" t="s">
         <v>33</v>
       </c>
@@ -3872,7 +3904,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
@@ -3896,7 +3928,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10">
@@ -3926,7 +3958,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="10" customFormat="1">
       <c r="D12" s="10" t="s">
         <v>37</v>
       </c>
@@ -3951,7 +3983,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="10" customFormat="1">
       <c r="D13" s="12">
         <v>5</v>
       </c>
@@ -3978,7 +4010,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -4001,7 +4033,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="12">
@@ -4028,7 +4060,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="12"/>
@@ -4051,7 +4083,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" ht="15.75" customHeight="1">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="12">
@@ -4078,7 +4110,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" ht="15.75" customHeight="1">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="12">
@@ -4107,7 +4139,7 @@
         <v>1793</v>
       </c>
     </row>
-    <row r="19" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" ht="15.75" customHeight="1">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="12"/>
@@ -4130,7 +4162,7 @@
         <v>1793</v>
       </c>
     </row>
-    <row r="20" spans="2:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" s="10" customFormat="1">
       <c r="D20" s="10" t="s">
         <v>42</v>
       </c>
@@ -4156,7 +4188,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="21" spans="2:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" s="10" customFormat="1">
       <c r="D21" s="10">
         <v>9</v>
       </c>
@@ -4181,7 +4213,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="22" spans="2:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" s="10" customFormat="1">
       <c r="D22" s="10" t="s">
         <v>42</v>
       </c>
@@ -4207,7 +4239,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="23" spans="2:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" s="10" customFormat="1">
       <c r="F23" s="10" t="s">
         <v>43</v>
       </c>
@@ -4226,7 +4258,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="24" spans="2:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" s="10" customFormat="1">
       <c r="D24" s="10">
         <v>10</v>
       </c>
@@ -4251,7 +4283,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="25" spans="2:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" s="10" customFormat="1">
       <c r="F25" s="10" t="s">
         <v>22</v>
       </c>
@@ -4270,7 +4302,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="26" spans="2:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" s="10" customFormat="1">
       <c r="F26" s="10" t="s">
         <v>30</v>
       </c>
@@ -4291,7 +4323,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="27" spans="2:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" s="10" customFormat="1">
       <c r="F27" s="10" t="s">
         <v>40</v>
       </c>
@@ -4310,7 +4342,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="28" spans="2:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" s="10" customFormat="1">
       <c r="D28" s="10">
         <v>11</v>
       </c>
@@ -4335,7 +4367,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="29" spans="2:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" s="10" customFormat="1">
       <c r="F29" s="10" t="s">
         <v>20</v>
       </c>
@@ -4354,7 +4386,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="30" spans="2:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" s="10" customFormat="1">
       <c r="F30" s="10" t="s">
         <v>2</v>
       </c>
@@ -4373,7 +4405,7 @@
         <v>2316</v>
       </c>
     </row>
-    <row r="31" spans="2:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" s="10" customFormat="1">
       <c r="F31" s="10" t="s">
         <v>46</v>
       </c>
@@ -4392,7 +4424,7 @@
         <v>1776</v>
       </c>
     </row>
-    <row r="32" spans="2:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" s="10" customFormat="1">
       <c r="D32" s="10">
         <v>12</v>
       </c>
@@ -4417,7 +4449,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="33" spans="2:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" s="10" customFormat="1">
       <c r="F33" s="10" t="s">
         <v>30</v>
       </c>
@@ -4436,30 +4468,32 @@
         <v>946</v>
       </c>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2">
+    <row r="34" spans="2:14" s="10" customFormat="1">
+      <c r="D34" s="10">
         <v>13</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F34" s="2"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
+      <c r="F34" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
       <c r="I34" s="11">
         <f t="shared" si="3"/>
         <v>5607</v>
       </c>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3">
-        <f t="shared" si="0"/>
-        <v>946</v>
-      </c>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J34" s="11"/>
+      <c r="K34" s="11">
+        <v>205</v>
+      </c>
+      <c r="L34" s="11">
+        <f t="shared" si="0"/>
+        <v>741</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2">
@@ -4483,10 +4517,10 @@
       <c r="K35" s="3"/>
       <c r="L35" s="3">
         <f t="shared" si="0"/>
-        <v>946</v>
-      </c>
-    </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14">
       <c r="D36" s="7">
         <v>15</v>
       </c>
@@ -4508,12 +4542,12 @@
       <c r="K36" s="3"/>
       <c r="L36" s="3">
         <f t="shared" si="0"/>
-        <v>946</v>
+        <v>741</v>
       </c>
       <c r="M36" s="7"/>
       <c r="N36" s="7"/>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14">
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7" t="s">
@@ -4531,12 +4565,12 @@
       <c r="K37" s="3"/>
       <c r="L37" s="3">
         <f t="shared" si="0"/>
-        <v>946</v>
+        <v>741</v>
       </c>
       <c r="M37" s="7"/>
       <c r="N37" s="7"/>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:14">
       <c r="D38" s="7">
         <v>16</v>
       </c>
@@ -4558,12 +4592,12 @@
       <c r="K38" s="3"/>
       <c r="L38" s="3">
         <f t="shared" si="0"/>
-        <v>946</v>
+        <v>741</v>
       </c>
       <c r="M38" s="7"/>
       <c r="N38" s="7"/>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14">
       <c r="D39" s="7">
         <v>17</v>
       </c>
@@ -4585,12 +4619,12 @@
       <c r="K39" s="3"/>
       <c r="L39" s="3">
         <f t="shared" si="0"/>
-        <v>946</v>
+        <v>741</v>
       </c>
       <c r="M39" s="7"/>
       <c r="N39" s="7"/>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14">
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
       <c r="F40" s="7" t="s">
@@ -4608,12 +4642,12 @@
       <c r="K40" s="3"/>
       <c r="L40" s="3">
         <f t="shared" si="0"/>
-        <v>946</v>
+        <v>741</v>
       </c>
       <c r="M40" s="7"/>
       <c r="N40" s="7"/>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:14">
       <c r="D41" s="7">
         <v>18</v>
       </c>
@@ -4635,12 +4669,12 @@
       <c r="K41" s="3"/>
       <c r="L41" s="3">
         <f t="shared" si="0"/>
-        <v>946</v>
+        <v>741</v>
       </c>
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14">
       <c r="D42" s="7">
         <v>19</v>
       </c>
@@ -4658,12 +4692,12 @@
       <c r="K42" s="3"/>
       <c r="L42" s="3">
         <f t="shared" si="0"/>
-        <v>946</v>
+        <v>741</v>
       </c>
       <c r="M42" s="7"/>
       <c r="N42" s="7"/>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:14">
       <c r="D43" s="7">
         <v>20</v>
       </c>
@@ -4681,12 +4715,12 @@
       <c r="K43" s="3"/>
       <c r="L43" s="3">
         <f t="shared" si="0"/>
-        <v>946</v>
+        <v>741</v>
       </c>
       <c r="M43" s="7"/>
       <c r="N43" s="7"/>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:14">
       <c r="D44" s="7">
         <v>21</v>
       </c>
@@ -4708,12 +4742,12 @@
       <c r="K44" s="3"/>
       <c r="L44" s="3">
         <f t="shared" si="0"/>
-        <v>946</v>
+        <v>741</v>
       </c>
       <c r="M44" s="7"/>
       <c r="N44" s="7"/>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:14">
       <c r="D45" s="7">
         <v>22</v>
       </c>
@@ -4735,12 +4769,12 @@
       <c r="K45" s="3"/>
       <c r="L45" s="3">
         <f t="shared" si="0"/>
-        <v>946</v>
+        <v>741</v>
       </c>
       <c r="M45" s="7"/>
       <c r="N45" s="7"/>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:14">
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
       <c r="F46" s="7" t="s">
@@ -4758,12 +4792,12 @@
       <c r="K46" s="3"/>
       <c r="L46" s="3">
         <f t="shared" si="0"/>
-        <v>946</v>
+        <v>741</v>
       </c>
       <c r="M46" s="7"/>
       <c r="N46" s="7"/>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:14">
       <c r="D47" s="7">
         <v>23</v>
       </c>
@@ -4785,12 +4819,12 @@
       <c r="K47" s="3"/>
       <c r="L47" s="3">
         <f t="shared" si="0"/>
-        <v>946</v>
+        <v>741</v>
       </c>
       <c r="M47" s="7"/>
       <c r="N47" s="7"/>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:14">
       <c r="D48" s="7">
         <v>24</v>
       </c>
@@ -4812,12 +4846,12 @@
       <c r="K48" s="3"/>
       <c r="L48" s="3">
         <f t="shared" si="0"/>
-        <v>946</v>
+        <v>741</v>
       </c>
       <c r="M48" s="7"/>
       <c r="N48" s="7"/>
     </row>
-    <row r="49" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:14">
       <c r="D49" s="7"/>
       <c r="E49" s="7"/>
       <c r="F49" s="7" t="s">
@@ -4835,12 +4869,12 @@
       <c r="K49" s="3"/>
       <c r="L49" s="3">
         <f t="shared" si="0"/>
-        <v>946</v>
+        <v>741</v>
       </c>
       <c r="M49" s="7"/>
       <c r="N49" s="7"/>
     </row>
-    <row r="50" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:14">
       <c r="D50" s="7"/>
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
@@ -4853,7 +4887,7 @@
       <c r="M50" s="7"/>
       <c r="N50" s="7"/>
     </row>
-    <row r="51" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:14">
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
@@ -4866,7 +4900,7 @@
       <c r="M51" s="7"/>
       <c r="N51" s="7"/>
     </row>
-    <row r="52" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:14">
       <c r="D52" s="7"/>
       <c r="E52" s="7"/>
       <c r="F52" s="7"/>
@@ -4879,7 +4913,7 @@
       <c r="M52" s="7"/>
       <c r="N52" s="7"/>
     </row>
-    <row r="53" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:14">
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
@@ -4892,7 +4926,7 @@
       <c r="M53" s="7"/>
       <c r="N53" s="7"/>
     </row>
-    <row r="54" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:14">
       <c r="D54" s="7"/>
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
@@ -4905,7 +4939,7 @@
       <c r="M54" s="7"/>
       <c r="N54" s="7"/>
     </row>
-    <row r="55" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:14">
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
       <c r="F55" s="7"/>
@@ -4918,7 +4952,7 @@
       <c r="M55" s="7"/>
       <c r="N55" s="7"/>
     </row>
-    <row r="56" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:14">
       <c r="D56" s="7"/>
       <c r="E56" s="7"/>
       <c r="F56" s="7"/>
@@ -4931,7 +4965,7 @@
       <c r="M56" s="7"/>
       <c r="N56" s="7"/>
     </row>
-    <row r="57" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:14">
       <c r="D57" s="7"/>
       <c r="E57" s="7"/>
       <c r="F57" s="7"/>
@@ -4944,7 +4978,7 @@
       <c r="M57" s="7"/>
       <c r="N57" s="7"/>
     </row>
-    <row r="58" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:14">
       <c r="D58" s="7"/>
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
@@ -4957,7 +4991,7 @@
       <c r="M58" s="7"/>
       <c r="N58" s="7"/>
     </row>
-    <row r="59" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:14">
       <c r="D59" s="7"/>
       <c r="E59" s="7"/>
       <c r="F59" s="7"/>
@@ -4970,7 +5004,7 @@
       <c r="M59" s="7"/>
       <c r="N59" s="7"/>
     </row>
-    <row r="60" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:14">
       <c r="D60" s="7"/>
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
@@ -4983,7 +5017,7 @@
       <c r="M60" s="7"/>
       <c r="N60" s="7"/>
     </row>
-    <row r="61" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:14">
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
       <c r="F61" s="7"/>
@@ -4996,7 +5030,7 @@
       <c r="M61" s="7"/>
       <c r="N61" s="7"/>
     </row>
-    <row r="62" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:14">
       <c r="D62" s="7"/>
       <c r="E62" s="7"/>
       <c r="F62" s="7"/>
@@ -5009,7 +5043,7 @@
       <c r="M62" s="7"/>
       <c r="N62" s="7"/>
     </row>
-    <row r="63" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:14">
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
       <c r="F63" s="7"/>
@@ -5022,7 +5056,7 @@
       <c r="M63" s="7"/>
       <c r="N63" s="7"/>
     </row>
-    <row r="64" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:14">
       <c r="D64" s="7"/>
       <c r="E64" s="7"/>
       <c r="F64" s="7"/>
@@ -5035,7 +5069,7 @@
       <c r="M64" s="7"/>
       <c r="N64" s="7"/>
     </row>
-    <row r="65" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:14">
       <c r="D65" s="7"/>
       <c r="E65" s="7"/>
       <c r="F65" s="7"/>
@@ -5048,7 +5082,7 @@
       <c r="M65" s="7"/>
       <c r="N65" s="7"/>
     </row>
-    <row r="66" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:14">
       <c r="D66" s="7"/>
       <c r="E66" s="7"/>
       <c r="F66" s="7"/>
@@ -5061,7 +5095,7 @@
       <c r="M66" s="7"/>
       <c r="N66" s="7"/>
     </row>
-    <row r="67" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:14">
       <c r="D67" s="7"/>
       <c r="E67" s="7"/>
       <c r="F67" s="7"/>
@@ -5074,7 +5108,7 @@
       <c r="M67" s="7"/>
       <c r="N67" s="7"/>
     </row>
-    <row r="68" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:14">
       <c r="D68" s="7"/>
       <c r="E68" s="7"/>
       <c r="F68" s="7"/>
@@ -5087,7 +5121,7 @@
       <c r="M68" s="7"/>
       <c r="N68" s="7"/>
     </row>
-    <row r="69" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:14">
       <c r="D69" s="7"/>
       <c r="E69" s="7"/>
       <c r="F69" s="7"/>
@@ -5100,7 +5134,7 @@
       <c r="M69" s="7"/>
       <c r="N69" s="7"/>
     </row>
-    <row r="70" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:14">
       <c r="D70" s="7"/>
       <c r="E70" s="7"/>
       <c r="F70" s="7"/>
@@ -5113,7 +5147,7 @@
       <c r="M70" s="7"/>
       <c r="N70" s="7"/>
     </row>
-    <row r="71" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:14">
       <c r="D71" s="7"/>
       <c r="E71" s="7"/>
       <c r="F71" s="7"/>
@@ -5126,7 +5160,7 @@
       <c r="M71" s="7"/>
       <c r="N71" s="7"/>
     </row>
-    <row r="72" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:14">
       <c r="D72" s="7"/>
       <c r="E72" s="7"/>
       <c r="F72" s="7"/>
@@ -5139,7 +5173,7 @@
       <c r="M72" s="7"/>
       <c r="N72" s="7"/>
     </row>
-    <row r="73" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:14">
       <c r="D73" s="7"/>
       <c r="E73" s="7"/>
       <c r="F73" s="7"/>
@@ -5152,7 +5186,7 @@
       <c r="M73" s="7"/>
       <c r="N73" s="7"/>
     </row>
-    <row r="74" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:14">
       <c r="D74" s="7"/>
       <c r="E74" s="7"/>
       <c r="F74" s="7"/>
@@ -5165,7 +5199,7 @@
       <c r="M74" s="7"/>
       <c r="N74" s="7"/>
     </row>
-    <row r="75" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:14">
       <c r="D75" s="7"/>
       <c r="E75" s="7"/>
       <c r="F75" s="7"/>
@@ -5178,7 +5212,7 @@
       <c r="M75" s="7"/>
       <c r="N75" s="7"/>
     </row>
-    <row r="76" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:14">
       <c r="D76" s="7"/>
       <c r="E76" s="7"/>
       <c r="F76" s="7"/>
@@ -5191,7 +5225,7 @@
       <c r="M76" s="7"/>
       <c r="N76" s="7"/>
     </row>
-    <row r="77" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:14">
       <c r="D77" s="7"/>
       <c r="E77" s="7"/>
       <c r="F77" s="7"/>
@@ -5204,7 +5238,7 @@
       <c r="M77" s="7"/>
       <c r="N77" s="7"/>
     </row>
-    <row r="78" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:14">
       <c r="D78" s="7"/>
       <c r="E78" s="7"/>
       <c r="F78" s="7"/>
@@ -5217,7 +5251,7 @@
       <c r="M78" s="7"/>
       <c r="N78" s="7"/>
     </row>
-    <row r="79" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:14">
       <c r="D79" s="7"/>
       <c r="E79" s="7"/>
       <c r="F79" s="7"/>
@@ -5230,7 +5264,7 @@
       <c r="M79" s="7"/>
       <c r="N79" s="7"/>
     </row>
-    <row r="80" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:14">
       <c r="D80" s="7"/>
       <c r="E80" s="7"/>
       <c r="F80" s="7"/>
@@ -5243,7 +5277,7 @@
       <c r="M80" s="7"/>
       <c r="N80" s="7"/>
     </row>
-    <row r="81" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:14">
       <c r="D81" s="7"/>
       <c r="E81" s="7"/>
       <c r="F81" s="7"/>
@@ -5256,7 +5290,7 @@
       <c r="M81" s="7"/>
       <c r="N81" s="7"/>
     </row>
-    <row r="82" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:14">
       <c r="D82" s="7"/>
       <c r="E82" s="7"/>
       <c r="F82" s="7"/>
@@ -5269,7 +5303,7 @@
       <c r="M82" s="7"/>
       <c r="N82" s="7"/>
     </row>
-    <row r="83" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:14">
       <c r="D83" s="7"/>
       <c r="E83" s="7"/>
       <c r="F83" s="7"/>
@@ -5282,7 +5316,7 @@
       <c r="M83" s="7"/>
       <c r="N83" s="7"/>
     </row>
-    <row r="84" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:14">
       <c r="D84" s="7"/>
       <c r="E84" s="7"/>
       <c r="F84" s="7"/>
@@ -5295,7 +5329,7 @@
       <c r="M84" s="7"/>
       <c r="N84" s="7"/>
     </row>
-    <row r="85" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:14">
       <c r="D85" s="7"/>
       <c r="E85" s="7"/>
       <c r="F85" s="7"/>
@@ -5308,7 +5342,7 @@
       <c r="M85" s="7"/>
       <c r="N85" s="7"/>
     </row>
-    <row r="86" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:14">
       <c r="D86" s="7"/>
       <c r="E86" s="7"/>
       <c r="F86" s="7"/>
@@ -5321,7 +5355,7 @@
       <c r="M86" s="7"/>
       <c r="N86" s="7"/>
     </row>
-    <row r="87" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="4:14">
       <c r="D87" s="7"/>
       <c r="E87" s="7"/>
       <c r="F87" s="7"/>
@@ -5334,7 +5368,7 @@
       <c r="M87" s="7"/>
       <c r="N87" s="7"/>
     </row>
-    <row r="88" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="4:14">
       <c r="D88" s="7"/>
       <c r="E88" s="7"/>
       <c r="F88" s="7"/>
@@ -5347,7 +5381,7 @@
       <c r="M88" s="7"/>
       <c r="N88" s="7"/>
     </row>
-    <row r="89" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="4:14">
       <c r="D89" s="7"/>
       <c r="E89" s="7"/>
       <c r="F89" s="7"/>
@@ -5360,7 +5394,7 @@
       <c r="M89" s="7"/>
       <c r="N89" s="7"/>
     </row>
-    <row r="90" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="4:14">
       <c r="D90" s="7"/>
       <c r="E90" s="7"/>
       <c r="F90" s="7"/>
@@ -5373,7 +5407,7 @@
       <c r="M90" s="7"/>
       <c r="N90" s="7"/>
     </row>
-    <row r="91" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="4:14">
       <c r="D91" s="7"/>
       <c r="E91" s="7"/>
       <c r="F91" s="7"/>
@@ -5386,7 +5420,7 @@
       <c r="M91" s="7"/>
       <c r="N91" s="7"/>
     </row>
-    <row r="92" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="4:14">
       <c r="D92" s="7"/>
       <c r="E92" s="7"/>
       <c r="F92" s="7"/>
@@ -5399,7 +5433,7 @@
       <c r="M92" s="7"/>
       <c r="N92" s="7"/>
     </row>
-    <row r="93" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="4:14">
       <c r="D93" s="7"/>
       <c r="E93" s="7"/>
       <c r="F93" s="7"/>
@@ -5412,7 +5446,7 @@
       <c r="M93" s="7"/>
       <c r="N93" s="7"/>
     </row>
-    <row r="94" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="4:14">
       <c r="D94" s="7"/>
       <c r="E94" s="7"/>
       <c r="F94" s="7"/>
@@ -5425,7 +5459,7 @@
       <c r="M94" s="7"/>
       <c r="N94" s="7"/>
     </row>
-    <row r="95" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="4:14">
       <c r="D95" s="7"/>
       <c r="E95" s="7"/>
       <c r="F95" s="7"/>
@@ -5438,7 +5472,7 @@
       <c r="M95" s="7"/>
       <c r="N95" s="7"/>
     </row>
-    <row r="96" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:14">
       <c r="D96" s="7"/>
       <c r="E96" s="7"/>
       <c r="F96" s="7"/>
@@ -5451,7 +5485,7 @@
       <c r="M96" s="7"/>
       <c r="N96" s="7"/>
     </row>
-    <row r="97" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="4:14">
       <c r="D97" s="7"/>
       <c r="E97" s="7"/>
       <c r="F97" s="7"/>
@@ -5464,7 +5498,7 @@
       <c r="M97" s="7"/>
       <c r="N97" s="7"/>
     </row>
-    <row r="98" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="4:14">
       <c r="D98" s="7"/>
       <c r="E98" s="7"/>
       <c r="F98" s="7"/>
@@ -5477,7 +5511,7 @@
       <c r="M98" s="7"/>
       <c r="N98" s="7"/>
     </row>
-    <row r="99" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="4:14">
       <c r="D99" s="7"/>
       <c r="E99" s="7"/>
       <c r="F99" s="7"/>
@@ -5490,7 +5524,7 @@
       <c r="M99" s="7"/>
       <c r="N99" s="7"/>
     </row>
-    <row r="100" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="4:14">
       <c r="D100" s="7"/>
       <c r="E100" s="7"/>
       <c r="F100" s="7"/>
@@ -5503,7 +5537,7 @@
       <c r="M100" s="7"/>
       <c r="N100" s="7"/>
     </row>
-    <row r="101" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="4:14">
       <c r="D101" s="7"/>
       <c r="E101" s="7"/>
       <c r="F101" s="7"/>
@@ -5516,7 +5550,7 @@
       <c r="M101" s="7"/>
       <c r="N101" s="7"/>
     </row>
-    <row r="102" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="4:14">
       <c r="D102" s="7"/>
       <c r="E102" s="7"/>
       <c r="F102" s="7"/>
@@ -5529,7 +5563,7 @@
       <c r="M102" s="7"/>
       <c r="N102" s="7"/>
     </row>
-    <row r="103" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="4:14">
       <c r="D103" s="7"/>
       <c r="E103" s="7"/>
       <c r="F103" s="7"/>
@@ -5542,7 +5576,7 @@
       <c r="M103" s="7"/>
       <c r="N103" s="7"/>
     </row>
-    <row r="104" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="104" spans="4:14">
       <c r="D104" s="7"/>
       <c r="E104" s="7"/>
       <c r="F104" s="7"/>
@@ -5555,7 +5589,7 @@
       <c r="M104" s="7"/>
       <c r="N104" s="7"/>
     </row>
-    <row r="105" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="105" spans="4:14">
       <c r="D105" s="7"/>
       <c r="E105" s="7"/>
       <c r="F105" s="7"/>
@@ -5568,7 +5602,7 @@
       <c r="M105" s="7"/>
       <c r="N105" s="7"/>
     </row>
-    <row r="106" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="106" spans="4:14">
       <c r="D106" s="7"/>
       <c r="E106" s="7"/>
       <c r="F106" s="7"/>
@@ -5581,7 +5615,7 @@
       <c r="M106" s="7"/>
       <c r="N106" s="7"/>
     </row>
-    <row r="107" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="107" spans="4:14">
       <c r="D107" s="7"/>
       <c r="E107" s="7"/>
       <c r="F107" s="7"/>
@@ -5594,7 +5628,7 @@
       <c r="M107" s="7"/>
       <c r="N107" s="7"/>
     </row>
-    <row r="108" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="108" spans="4:14">
       <c r="D108" s="7"/>
       <c r="E108" s="7"/>
       <c r="F108" s="7"/>
@@ -5607,7 +5641,7 @@
       <c r="M108" s="7"/>
       <c r="N108" s="7"/>
     </row>
-    <row r="109" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="109" spans="4:14">
       <c r="D109" s="7"/>
       <c r="E109" s="7"/>
       <c r="F109" s="7"/>
@@ -5620,7 +5654,7 @@
       <c r="M109" s="7"/>
       <c r="N109" s="7"/>
     </row>
-    <row r="110" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="110" spans="4:14">
       <c r="D110" s="7"/>
       <c r="E110" s="7"/>
       <c r="F110" s="7"/>
@@ -5633,7 +5667,7 @@
       <c r="M110" s="7"/>
       <c r="N110" s="7"/>
     </row>
-    <row r="111" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="111" spans="4:14">
       <c r="D111" s="7"/>
       <c r="E111" s="7"/>
       <c r="F111" s="7"/>
@@ -5646,7 +5680,7 @@
       <c r="M111" s="7"/>
       <c r="N111" s="7"/>
     </row>
-    <row r="112" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="112" spans="4:14">
       <c r="D112" s="7"/>
       <c r="E112" s="7"/>
       <c r="F112" s="7"/>
@@ -5659,7 +5693,7 @@
       <c r="M112" s="7"/>
       <c r="N112" s="7"/>
     </row>
-    <row r="113" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="113" spans="4:14">
       <c r="D113" s="7"/>
       <c r="E113" s="7"/>
       <c r="F113" s="7"/>
@@ -5672,7 +5706,7 @@
       <c r="M113" s="7"/>
       <c r="N113" s="7"/>
     </row>
-    <row r="114" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="114" spans="4:14">
       <c r="D114" s="7"/>
       <c r="E114" s="7"/>
       <c r="F114" s="7"/>

</xml_diff>